<commit_message>
Documentation of SKOS Play convert
</commit_message>
<xml_diff>
--- a/fr.sparna/rdf/skos/skos-play/src/main/webapp/excel_test/excel2skos-exemple-4.xlsx
+++ b/fr.sparna/rdf/skos/skos-play/src/main/webapp/excel_test/excel2skos-exemple-4.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="25">
   <si>
     <t>URI</t>
   </si>
@@ -87,6 +87,9 @@
   </si>
   <si>
     <t>schema:location</t>
+  </si>
+  <si>
+    <t>schema:startDate^^xsd:date</t>
   </si>
 </sst>
 </file>
@@ -147,7 +150,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -161,6 +164,7 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
@@ -456,10 +460,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -469,9 +473,10 @@
     <col min="3" max="3" width="26.7109375" customWidth="1"/>
     <col min="4" max="4" width="21" style="1" customWidth="1"/>
     <col min="5" max="5" width="17.28515625" customWidth="1"/>
+    <col min="6" max="6" width="31.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="A1" s="5" t="s">
         <v>2</v>
       </c>
@@ -479,7 +484,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:6">
       <c r="A2" s="5" t="s">
         <v>1</v>
       </c>
@@ -490,7 +495,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:6">
       <c r="A3" s="5" t="s">
         <v>1</v>
       </c>
@@ -501,16 +506,16 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:6">
       <c r="A4" s="5"/>
       <c r="C4" s="6"/>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:6">
       <c r="A5" s="5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:6">
       <c r="A7" s="3" t="s">
         <v>0</v>
       </c>
@@ -526,8 +531,11 @@
       <c r="E7" s="3" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="8" spans="1:5">
+      <c r="F7" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -543,8 +551,11 @@
       <c r="E8" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="9" spans="1:5">
+      <c r="F8" s="7">
+        <v>42695</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -560,20 +571,23 @@
       <c r="E9" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="10" spans="1:5">
+      <c r="F9" s="7">
+        <v>42519</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
       <c r="C10" s="1"/>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:6">
       <c r="C11" s="1"/>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:6">
       <c r="C12" s="1"/>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:6">
       <c r="C13" s="1"/>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:6">
       <c r="A14" s="2"/>
       <c r="C14" s="1"/>
     </row>
@@ -637,7 +651,7 @@
     <row r="5" spans="1:4">
       <c r="D5" s="1"/>
     </row>
-    <row r="6" spans="1:4" ht="30">
+    <row r="6" spans="1:4">
       <c r="A6" s="3" t="s">
         <v>0</v>
       </c>

</xml_diff>